<commit_message>
Risistemato l'ordine di euristici e ricerche locali per rispecchiare quanto deciso
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_post.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_post.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R90"/>
+  <dimension ref="A1:S90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,41 +515,41 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251455</v>
+        <v>251742</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D2" t="n">
-        <v>82.765625</v>
+        <v>134.8524590163935</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-05-07 07:00:00</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-07 08:41:45</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>5297</v>
+        <v>8226</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -580,50 +580,53 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025-04-15 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R2" s="1" t="n">
-        <v>-0.3623372395833334</v>
+        <v>-1.406147540983796</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>-1.406147540983796</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251391</v>
+        <v>251840</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D3" t="n">
-        <v>91.640625</v>
+        <v>93.67213114754098</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-07 08:41:45</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-07 08:58:45</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-07 08:58:45</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-07 10:30:24</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>5865</v>
+        <v>5714</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -642,7 +645,7 @@
         <v>70</v>
       </c>
       <c r="N3" t="n">
-        <v>39749</v>
+        <v>39758</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -650,54 +653,57 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>39749</v>
+        <v>39758</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-0.4377821180555556</v>
+        <v>-0.4885587431712963</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>-0.4885587431712963</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251395</v>
+        <v>251456</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D4" t="n">
-        <v>35.34375</v>
+        <v>147.5245901639344</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-07 10:30:24</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-07 10:47:24</t>
+          <t>2025-05-08 12:13:31</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-07 10:47:24</t>
+          <t>2025-05-08 12:13:31</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:45</t>
+          <t>2025-05-08 14:41:02</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>2262</v>
+        <v>8999</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -710,13 +716,13 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M4" t="n">
         <v>70</v>
       </c>
       <c r="N4" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -724,54 +730,57 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R4" s="1" t="n">
-        <v>-0.4741319444444445</v>
+        <v>-2.611839708564815</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>-2.611839708564815</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251371</v>
+        <v>251284</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>19</v>
+        <v>40.5</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:45</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>16340</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -780,19 +789,17 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M5" t="n">
         <v>70</v>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>39666 (esterno)</t>
-        </is>
+      <c r="N5" t="n">
+        <v>39747</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -800,74 +807,77 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>39666</v>
+        <v>39747</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-04-24 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R5" s="1" t="n">
-        <v>-13.48732638888889</v>
+        <v>-1.526104797974537</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <v>-1.526104797974537</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251453</v>
+        <v>251706</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>78.125</v>
+        <v>50.79365079365079</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-07 11:58:45</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-07 11:58:45</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-07 13:16:52</t>
+          <t>2025-05-12 07:50:47</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>5000</v>
+        <v>3200</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>bobina</t>
+          <t>foglio</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>39742 (non in estrazione)</t>
+          <t>39764 (esterno)</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -876,20 +886,23 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>39742</v>
+        <v>39764</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-05-14 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251396</v>
+        <v>251455</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -897,33 +910,33 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" t="n">
-        <v>35.34375</v>
+        <v>82.765625</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-07 13:16:52</t>
+          <t>2025-05-07 07:00:00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-07 13:37:52</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-07 13:37:52</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-07 14:13:13</t>
+          <t>2025-05-07 08:41:45</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>2262</v>
+        <v>5297</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -936,7 +949,7 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M7" t="n">
         <v>70</v>
@@ -954,16 +967,19 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
+          <t>2025-04-15 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-0.5925130208333333</v>
+        <v>-0.3623372395833334</v>
+      </c>
+      <c r="S7" s="1" t="n">
+        <v>-0.3623372395833334</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251548</v>
+        <v>251391</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -971,33 +987,33 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" t="n">
-        <v>206.90625</v>
+        <v>91.640625</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-07 14:13:13</t>
+          <t>2025-05-07 08:41:45</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-07 14:32:13</t>
+          <t>2025-05-07 08:58:45</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-07 14:32:13</t>
+          <t>2025-05-07 08:58:45</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-08 09:59:07</t>
+          <t>2025-05-07 10:30:24</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>13242</v>
+        <v>5865</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1010,7 +1026,7 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M8" t="n">
         <v>70</v>
@@ -1028,50 +1044,53 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>-1.416059027777778</v>
+        <v>-0.4377821180555556</v>
+      </c>
+      <c r="S8" s="1" t="n">
+        <v>-0.4377821180555556</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251547</v>
+        <v>251395</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D9" t="n">
-        <v>184.9154929577465</v>
+        <v>35.34375</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-07 10:30:24</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-07 10:47:24</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-07 10:47:24</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-07 11:22:45</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>13129</v>
+        <v>2262</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1084,7 +1103,7 @@
         </is>
       </c>
       <c r="L9" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M9" t="n">
         <v>70</v>
@@ -1102,50 +1121,53 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>-0.4741319444444445</v>
+      </c>
+      <c r="S9" s="1" t="n">
+        <v>-0.4741319444444445</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251742</v>
+        <v>251371</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D10" t="n">
-        <v>134.8524590163935</v>
+        <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-07 11:22:45</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>8226</v>
+        <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1163,8 +1185,10 @@
       <c r="M10" t="n">
         <v>70</v>
       </c>
-      <c r="N10" t="n">
-        <v>39749</v>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>39666 (esterno)</t>
+        </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1172,54 +1196,57 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>39749</v>
+        <v>39666</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-24 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-13.48732638888889</v>
+      </c>
+      <c r="S10" s="1" t="n">
+        <v>-13.48732638888889</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251268</v>
+        <v>251396</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>35.34375</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-07 12:00:45</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-07 12:00:45</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-07 12:36:05</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>2262</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1228,19 +1255,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M11" t="n">
-        <v>76</v>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>39666 (non in estrazione)</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="N11" t="n">
+        <v>39749</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1248,54 +1273,57 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39666</v>
+        <v>39749</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-04-14 00:00:00</t>
+          <t>2025-05-02 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>0</v>
+        <v>-0.5925130208333333</v>
+      </c>
+      <c r="S11" s="1" t="n">
+        <v>-0.5250651041666666</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251164</v>
+        <v>251548</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="D12" t="n">
-        <v>204.0816326530612</v>
+        <v>206.90625</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-07 12:36:05</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-08 08:34:00</t>
+          <t>2025-05-07 12:55:05</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-08 08:34:00</t>
+          <t>2025-05-07 12:55:05</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-08 11:58:04</t>
+          <t>2025-05-08 08:22:00</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>10000</v>
+        <v>13242</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1308,7 +1336,7 @@
         </is>
       </c>
       <c r="L12" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M12" t="n">
         <v>70</v>
@@ -1326,50 +1354,53 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>-1.498667800451389</v>
+        <v>-1.416059027777778</v>
+      </c>
+      <c r="S12" s="1" t="n">
+        <v>-1.348611111111111</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251840</v>
+        <v>251268</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D13" t="n">
-        <v>93.67213114754098</v>
+        <v>0</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-08 08:22:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-08 08:52:00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-08 08:52:00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-08 08:52:00</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>5714</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1378,17 +1409,19 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M13" t="n">
-        <v>70</v>
-      </c>
-      <c r="N13" t="n">
-        <v>39758</v>
+        <v>76</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>39666 (non in estrazione)</t>
+        </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1396,15 +1429,18 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39758</v>
+        <v>39666</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-04-14 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>0</v>
+      </c>
+      <c r="S13" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1417,29 +1453,29 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D14" t="n">
         <v>109.46875</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-08 09:59:07</t>
+          <t>2025-05-08 08:52:00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-08 10:31:07</t>
+          <t>2025-05-08 09:09:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-08 10:31:07</t>
+          <t>2025-05-08 09:09:00</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-08 12:20:35</t>
+          <t>2025-05-08 10:58:28</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1480,44 +1516,47 @@
       <c r="R14" s="1" t="n">
         <v>-1.514301215277778</v>
       </c>
+      <c r="S14" s="1" t="n">
+        <v>-1.457269965277778</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>250759</v>
+        <v>251225</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D15" t="n">
-        <v>118.2816901408451</v>
+        <v>0</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-08 10:58:28</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-08 11:15:28</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-08 11:15:28</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-08 11:15:28</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>8398</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1526,7 +1565,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L15" t="n">
@@ -1548,50 +1587,53 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-0.5261067708333333</v>
+      </c>
+      <c r="S15" s="1" t="n">
+        <v>-0.4690755208333333</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251456</v>
+        <v>251227</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>147.5245901639344</v>
+        <v>0</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-08 11:15:28</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-08 12:13:31</t>
+          <t>2025-05-08 11:30:28</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-08 12:13:31</t>
+          <t>2025-05-08 11:30:28</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-08 14:41:02</t>
+          <t>2025-05-08 11:30:28</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>8999</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1600,14 +1642,14 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M16" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N16" t="n">
         <v>39746</v>
@@ -1622,50 +1664,53 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-2.611839708564815</v>
+        <v>-2.5365234375</v>
+      </c>
+      <c r="S16" s="1" t="n">
+        <v>-2.4794921875</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251477</v>
+        <v>251421</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C17" t="n">
         <v>17</v>
       </c>
       <c r="D17" t="n">
-        <v>422.5211267605634</v>
+        <v>81.9375</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-08 11:30:28</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-08 12:17:00</t>
+          <t>2025-05-08 11:47:28</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-08 12:17:00</t>
+          <t>2025-05-08 11:47:28</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-09 11:19:31</t>
+          <t>2025-05-08 13:09:24</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>29999</v>
+        <v>5244</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1683,8 +1728,10 @@
       <c r="M17" t="n">
         <v>76</v>
       </c>
-      <c r="N17" t="n">
-        <v>39760</v>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>39762 (non in estrazione)</t>
+        </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1692,20 +1739,23 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>39760</v>
+        <v>39762</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-05-08 00:00:00</t>
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>-2.471889671365741</v>
+        <v>0</v>
+      </c>
+      <c r="S17" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251225</v>
+        <v>251782</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1713,33 +1763,33 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>188.640625</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-08 12:20:35</t>
+          <t>2025-05-08 13:09:24</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-08 13:24:24</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-08 13:24:24</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-09 08:33:02</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>12073</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1748,17 +1798,17 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M18" t="n">
         <v>76</v>
       </c>
       <c r="N18" t="n">
-        <v>39747</v>
+        <v>39754</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1766,54 +1816,57 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>39747</v>
+        <v>39754</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>-0.5261067708333333</v>
+        <v>-0.4133138020833333</v>
+      </c>
+      <c r="S18" s="1" t="n">
+        <v>-0.3562825520833333</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251227</v>
+        <v>251547</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>13129</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1822,17 +1875,17 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L19" t="n">
         <v>4</v>
       </c>
       <c r="M19" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N19" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1840,54 +1893,57 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R19" s="1" t="n">
-        <v>-2.5365234375</v>
+        <v>-1.443691314548611</v>
+      </c>
+      <c r="S19" s="1" t="n">
+        <v>-1.443691314548611</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251421</v>
+        <v>250759</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D20" t="n">
-        <v>81.9375</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-08 13:09:35</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-08 13:09:35</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-08 14:31:31</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>5244</v>
+        <v>8398</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1896,19 +1952,17 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M20" t="n">
         <v>76</v>
       </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>39762 (non in estrazione)</t>
-        </is>
+      <c r="N20" t="n">
+        <v>39747</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1916,20 +1970,23 @@
         </is>
       </c>
       <c r="P20" t="n">
-        <v>39762</v>
+        <v>39747</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2025-05-08 00:00:00</t>
+          <t>2025-03-13 00:00:00</t>
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>0</v>
+        <v>-0.5466647104861111</v>
+      </c>
+      <c r="S20" s="1" t="n">
+        <v>-0.5466647104861111</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251229</v>
+        <v>251416</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1940,7 +1997,7 @@
         <v>34</v>
       </c>
       <c r="D21" t="n">
-        <v>263.9295774647887</v>
+        <v>158.056338028169</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1959,11 +2016,11 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-09 10:05:07</t>
+          <t>2025-05-09 08:19:15</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>18739</v>
+        <v>11222</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1972,74 +2029,73 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M21" t="n">
         <v>70</v>
       </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>39723 (esterno)</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="N21" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
       </c>
       <c r="P21" t="n">
-        <v>39723</v>
+        <v>0</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>251782</v>
+        <v>251453</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D22" t="n">
-        <v>188.640625</v>
+        <v>70.4225352112676</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-08 14:31:31</t>
+          <t>2025-05-09 08:19:15</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-08 14:46:31</t>
+          <t>2025-05-09 08:36:15</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-08 14:46:31</t>
+          <t>2025-05-09 08:36:15</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-09 09:55:10</t>
+          <t>2025-05-09 09:46:40</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>12073</v>
+        <v>5000</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2048,17 +2104,19 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L22" t="n">
         <v>3</v>
       </c>
       <c r="M22" t="n">
-        <v>76</v>
-      </c>
-      <c r="N22" t="n">
-        <v>39754</v>
+        <v>70</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>39742 (non in estrazione)</t>
+        </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2066,54 +2124,57 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>39754</v>
+        <v>39742</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>-0.4133138020833333</v>
+        <v>0</v>
+      </c>
+      <c r="S22" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251284</v>
+        <v>251229</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>40.5</v>
+        <v>21</v>
       </c>
       <c r="D23" t="n">
-        <v>297.0909090909091</v>
+        <v>263.9295774647887</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-09 09:46:40</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-09 10:07:40</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-09 10:07:40</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-09 14:31:36</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>16340</v>
+        <v>18739</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2122,17 +2183,19 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M23" t="n">
         <v>70</v>
       </c>
-      <c r="N23" t="n">
-        <v>39747</v>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2140,15 +2203,18 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>39747</v>
+        <v>39723</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>0</v>
+      </c>
+      <c r="S23" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -2224,6 +2290,9 @@
       <c r="R24" s="1" t="n">
         <v>-1.442361111111111</v>
       </c>
+      <c r="S24" s="1" t="n">
+        <v>-1.442361111111111</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2298,6 +2367,9 @@
       <c r="R25" s="1" t="n">
         <v>-1.466666666666667</v>
       </c>
+      <c r="S25" s="1" t="n">
+        <v>-1.466666666666667</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2374,65 +2446,66 @@
       <c r="R26" s="1" t="n">
         <v>-16.58293231612268</v>
       </c>
+      <c r="S26" s="1" t="n">
+        <v>-16.58293231612268</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251706</v>
+        <v>251477</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D27" t="n">
-        <v>50.79365079365079</v>
+        <v>422.5211267605634</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 12:17:00</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 12:17:00</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-12 07:50:47</t>
+          <t>2025-05-09 11:19:31</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>3200</v>
+        <v>29999</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>foglio</t>
+          <t>bobina</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" t="inlineStr">
-        <is>
-          <t>39764 (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N27" t="n">
+        <v>39760</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2440,20 +2513,23 @@
         </is>
       </c>
       <c r="P27" t="n">
-        <v>39764</v>
+        <v>39760</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>2025-05-14 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R27" s="1" t="n">
-        <v>0</v>
+        <v>-2.471889671365741</v>
+      </c>
+      <c r="S27" s="1" t="n">
+        <v>-2.471889671365741</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>250894</v>
+        <v>251164</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2461,33 +2537,33 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="D28" t="n">
-        <v>903.3061224489796</v>
+        <v>204.0816326530612</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-05-08 11:58:04</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-05-08 12:40:04</t>
+          <t>2025-05-08 07:55:00</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-05-08 12:40:04</t>
+          <t>2025-05-08 07:55:00</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-05-12 11:43:23</t>
+          <t>2025-05-08 11:19:04</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>44262</v>
+        <v>10000</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2496,70 +2572,75 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L28" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M28" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N28" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O28" t="n">
-        <v>0</v>
+        <v>39749</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P28" t="n">
-        <v>0</v>
+        <v>39749</v>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-22 00:00:00</t>
         </is>
       </c>
       <c r="R28" s="1" t="n">
-        <v>0</v>
+        <v>-1.498667800451389</v>
+      </c>
+      <c r="S28" s="1" t="n">
+        <v>-1.471584467118056</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>251416</v>
+        <v>250894</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D29" t="n">
-        <v>183.9672131147541</v>
+        <v>903.3061224489796</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-05-08 14:41:02</t>
+          <t>2025-05-08 11:19:04</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-05-09 07:06:02</t>
+          <t>2025-05-08 12:01:04</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-05-09 07:06:02</t>
+          <t>2025-05-08 12:01:04</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-05-09 10:10:00</t>
+          <t>2025-05-12 11:04:23</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>11222</v>
+        <v>44262</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2568,14 +2649,14 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L29" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M29" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N29" t="n">
         <v>39755</v>
@@ -2588,10 +2669,13 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2664,6 +2748,9 @@
         </is>
       </c>
       <c r="R30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tolti import inutili, messo quello utile
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_post.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_post.xlsx
@@ -515,41 +515,41 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251455</v>
+        <v>251547</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D2" t="n">
-        <v>82.765625</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-05-07 07:00:00</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-07 08:41:45</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>5297</v>
+        <v>13129</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -580,53 +580,53 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025-04-15 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R2" s="1" t="n">
-        <v>-0.3623372395833334</v>
+        <v>-1.443691314548611</v>
       </c>
       <c r="S2" s="1" t="n">
-        <v>-0.3623372395833334</v>
+        <v>-1.443691314548611</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251391</v>
+        <v>250759</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D3" t="n">
-        <v>91.640625</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-07 08:41:45</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-07 08:58:45</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-07 08:58:45</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-07 10:30:24</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>5865</v>
+        <v>8398</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -635,17 +635,17 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M3" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N3" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -653,57 +653,57 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-03-13 00:00:00</t>
         </is>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-0.4377821180555556</v>
+        <v>-0.5466647104861111</v>
       </c>
       <c r="S3" s="1" t="n">
-        <v>-0.4377821180555556</v>
+        <v>-0.5466647104861111</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251395</v>
+        <v>251229</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D4" t="n">
-        <v>35.34375</v>
+        <v>263.9295774647887</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-07 10:30:24</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-07 10:47:24</t>
+          <t>2025-05-08 13:41:11</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-07 10:47:24</t>
+          <t>2025-05-08 13:41:11</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:45</t>
+          <t>2025-05-09 10:05:07</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>2262</v>
+        <v>18739</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -712,7 +712,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L4" t="n">
@@ -721,8 +721,10 @@
       <c r="M4" t="n">
         <v>70</v>
       </c>
-      <c r="N4" t="n">
-        <v>39749</v>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -730,57 +732,57 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>39749</v>
+        <v>39723</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R4" s="1" t="n">
-        <v>-0.4741319444444445</v>
+        <v>0</v>
       </c>
       <c r="S4" s="1" t="n">
-        <v>-0.4741319444444445</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251371</v>
+        <v>251416</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>158.056338028169</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:45</t>
+          <t>2025-05-09 10:05:07</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-09 10:28:07</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-09 10:28:07</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-09 13:06:10</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>11222</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -793,73 +795,69 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M5" t="n">
         <v>70</v>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>39666 (esterno)</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="N5" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>39666</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-04-24 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R5" s="1" t="n">
-        <v>-13.48732638888889</v>
+        <v>0</v>
       </c>
       <c r="S5" s="1" t="n">
-        <v>-13.48732638888889</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251453</v>
+        <v>251742</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D6" t="n">
-        <v>78.125</v>
+        <v>134.8524590163935</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-07 11:58:45</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-07 11:58:45</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-07 13:16:52</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>5000</v>
+        <v>8226</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -872,15 +870,13 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M6" t="n">
         <v>70</v>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>39742 (non in estrazione)</t>
-        </is>
+      <c r="N6" t="n">
+        <v>39749</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -888,57 +884,57 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>39742</v>
+        <v>39749</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-9.553385416666666</v>
+        <v>-1.406147540983796</v>
       </c>
       <c r="S6" s="1" t="n">
-        <v>-9.553385416666666</v>
+        <v>-1.406147540983796</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251396</v>
+        <v>251840</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D7" t="n">
-        <v>35.34375</v>
+        <v>93.67213114754098</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-07 13:16:52</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-07 13:37:52</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-07 13:37:52</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-07 14:13:13</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>2262</v>
+        <v>5714</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -951,13 +947,13 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M7" t="n">
         <v>70</v>
       </c>
       <c r="N7" t="n">
-        <v>39749</v>
+        <v>39758</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -965,57 +961,57 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>39749</v>
+        <v>39758</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-0.5925130208333333</v>
+        <v>-0.4885587431712963</v>
       </c>
       <c r="S7" s="1" t="n">
-        <v>-0.5925130208333333</v>
+        <v>-0.4885587431712963</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251548</v>
+        <v>251456</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D8" t="n">
-        <v>206.90625</v>
+        <v>147.5245901639344</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-07 14:13:13</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-07 14:32:13</t>
+          <t>2025-05-08 12:13:31</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-07 14:32:13</t>
+          <t>2025-05-08 12:13:31</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-08 09:59:07</t>
+          <t>2025-05-08 14:41:02</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>13242</v>
+        <v>8999</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1028,13 +1024,13 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M8" t="n">
         <v>70</v>
       </c>
       <c r="N8" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1042,57 +1038,57 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>-1.416059027777778</v>
+        <v>-2.611839708564815</v>
       </c>
       <c r="S8" s="1" t="n">
-        <v>-1.416059027777778</v>
+        <v>-2.611839708564815</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>250923</v>
+        <v>251477</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D9" t="n">
-        <v>109.46875</v>
+        <v>422.5211267605634</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-08 09:59:07</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-08 10:31:07</t>
+          <t>2025-05-08 12:17:00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-08 10:31:07</t>
+          <t>2025-05-08 12:17:00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-08 12:20:35</t>
+          <t>2025-05-09 11:19:31</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>7006</v>
+        <v>29999</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1101,17 +1097,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M9" t="n">
         <v>76</v>
       </c>
       <c r="N9" t="n">
-        <v>39749</v>
+        <v>39760</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1119,53 +1115,53 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>39749</v>
+        <v>39760</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-1.514301215277778</v>
+        <v>-2.471889671365741</v>
       </c>
       <c r="S9" s="1" t="n">
-        <v>-1.514301215277778</v>
+        <v>-2.471889671365741</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251225</v>
+        <v>251268</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-05-08 12:20:35</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-08 07:47:00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-08 07:47:00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-08 07:47:00</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1178,7 +1174,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L10" t="n">
@@ -1187,8 +1183,10 @@
       <c r="M10" t="n">
         <v>76</v>
       </c>
-      <c r="N10" t="n">
-        <v>39747</v>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>39666 (non in estrazione)</t>
+        </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1196,57 +1194,57 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>39747</v>
+        <v>39666</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-04-14 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-0.5261067708333333</v>
+        <v>-24.32430555555555</v>
       </c>
       <c r="S10" s="1" t="n">
-        <v>-0.5261067708333333</v>
+        <v>-24.32430555555555</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251227</v>
+        <v>251164</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>204.0816326530612</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-08 07:47:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-08 08:34:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-08 08:34:00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-08 11:58:04</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1255,17 +1253,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M11" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N11" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1273,23 +1271,23 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-22 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-2.5365234375</v>
+        <v>-1.498667800451389</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>-2.5365234375</v>
+        <v>-1.498667800451389</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251421</v>
+        <v>251455</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1297,33 +1295,33 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D12" t="n">
-        <v>81.9375</v>
+        <v>82.765625</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-07 07:00:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-08 13:09:35</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-08 13:09:35</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-08 14:31:31</t>
+          <t>2025-05-07 08:41:45</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>5244</v>
+        <v>5297</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1332,19 +1330,17 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M12" t="n">
-        <v>76</v>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>39762 (non in estrazione)</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="N12" t="n">
+        <v>39749</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1352,23 +1348,23 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>39762</v>
+        <v>39749</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-05-08 00:00:00</t>
+          <t>2025-04-15 00:00:00</t>
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>-0.6052300347222223</v>
+        <v>-0.3623372395833334</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>-0.6052300347222223</v>
+        <v>-0.3623372395833334</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251782</v>
+        <v>251391</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1376,33 +1372,33 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D13" t="n">
-        <v>188.640625</v>
+        <v>91.640625</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-08 14:31:31</t>
+          <t>2025-05-07 08:41:45</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-08 14:46:31</t>
+          <t>2025-05-07 08:58:45</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-08 14:46:31</t>
+          <t>2025-05-07 08:58:45</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-09 09:55:10</t>
+          <t>2025-05-07 10:30:24</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>12073</v>
+        <v>5865</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1411,17 +1407,17 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M13" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N13" t="n">
-        <v>39754</v>
+        <v>39749</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1429,23 +1425,23 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39754</v>
+        <v>39749</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-0.4133138020833333</v>
+        <v>-0.4377821180555556</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>-0.4133138020833333</v>
+        <v>-0.4377821180555556</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>250894</v>
+        <v>251395</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1453,33 +1449,33 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D14" t="n">
-        <v>691.59375</v>
+        <v>35.34375</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-09 09:55:10</t>
+          <t>2025-05-07 10:30:24</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-09 10:14:10</t>
+          <t>2025-05-07 10:47:24</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-09 10:14:10</t>
+          <t>2025-05-07 10:47:24</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-12 13:45:45</t>
+          <t>2025-05-07 11:22:45</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>44262</v>
+        <v>2262</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1488,73 +1484,75 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M14" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N14" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
+        <v>39749</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>39749</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>0</v>
+        <v>-0.4741319444444445</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0</v>
+        <v>-0.4741319444444445</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>251284</v>
+        <v>251371</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>40.5</v>
+        <v>19</v>
       </c>
       <c r="D15" t="n">
-        <v>297.0909090909091</v>
+        <v>0</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-07 11:22:45</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>16340</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1563,17 +1561,19 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M15" t="n">
         <v>70</v>
       </c>
-      <c r="N15" t="n">
-        <v>39747</v>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>39666 (esterno)</t>
+        </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1581,57 +1581,57 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>39747</v>
+        <v>39666</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-04-24 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>-13.48732638888889</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>-13.48732638888889</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251547</v>
+        <v>251453</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D16" t="n">
-        <v>184.9154929577465</v>
+        <v>78.125</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-07 11:58:45</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-07 11:58:45</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-07 13:16:52</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>13129</v>
+        <v>5000</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1644,13 +1644,15 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M16" t="n">
         <v>70</v>
       </c>
-      <c r="N16" t="n">
-        <v>39749</v>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>39742 (non in estrazione)</t>
+        </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1658,57 +1660,57 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>39749</v>
+        <v>39742</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>-9.553385416666666</v>
       </c>
       <c r="S16" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>-9.553385416666666</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>250759</v>
+        <v>251396</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D17" t="n">
-        <v>118.2816901408451</v>
+        <v>35.34375</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-07 13:16:52</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-07 13:37:52</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-07 13:37:52</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-07 14:13:13</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>8398</v>
+        <v>2262</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1717,17 +1719,17 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M17" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N17" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1735,57 +1737,57 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
+          <t>2025-05-02 00:00:00</t>
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-0.5925130208333333</v>
       </c>
       <c r="S17" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-0.5925130208333333</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251229</v>
+        <v>251548</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D18" t="n">
-        <v>263.9295774647887</v>
+        <v>206.90625</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-07 14:13:13</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-08 13:41:11</t>
+          <t>2025-05-07 14:32:13</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-08 13:41:11</t>
+          <t>2025-05-07 14:32:13</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-09 10:05:07</t>
+          <t>2025-05-08 09:59:07</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>18739</v>
+        <v>13242</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1794,19 +1796,17 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M18" t="n">
         <v>70</v>
       </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>39723 (esterno)</t>
-        </is>
+      <c r="N18" t="n">
+        <v>39749</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1814,57 +1814,57 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>39723</v>
+        <v>39749</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>0</v>
+        <v>-1.416059027777778</v>
       </c>
       <c r="S18" s="1" t="n">
-        <v>0</v>
+        <v>-1.416059027777778</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251416</v>
+        <v>250923</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D19" t="n">
-        <v>158.056338028169</v>
+        <v>109.46875</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-09 10:05:07</t>
+          <t>2025-05-08 09:59:07</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-09 10:28:07</t>
+          <t>2025-05-08 10:31:07</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-09 10:28:07</t>
+          <t>2025-05-08 10:31:07</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-09 13:06:10</t>
+          <t>2025-05-08 12:20:35</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>11222</v>
+        <v>7006</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1873,94 +1873,94 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M19" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N19" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O19" t="n">
-        <v>0</v>
+        <v>39749</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P19" t="n">
-        <v>0</v>
+        <v>39749</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-07 00:00:00</t>
         </is>
       </c>
       <c r="R19" s="1" t="n">
-        <v>0</v>
+        <v>-1.514301215277778</v>
       </c>
       <c r="S19" s="1" t="n">
-        <v>0</v>
+        <v>-1.514301215277778</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251706</v>
+        <v>251225</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D20" t="n">
-        <v>50.79365079365079</v>
+        <v>0</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 12:20:35</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 12:37:35</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 12:37:35</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-12 07:50:47</t>
+          <t>2025-05-08 12:37:35</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>foglio</t>
+          <t>bobina</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M20" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>39764 (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N20" t="n">
+        <v>39747</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1968,57 +1968,57 @@
         </is>
       </c>
       <c r="P20" t="n">
-        <v>39764</v>
+        <v>39747</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2025-05-14 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>0</v>
+        <v>-0.5261067708333333</v>
       </c>
       <c r="S20" s="1" t="n">
-        <v>0</v>
+        <v>-0.5261067708333333</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251477</v>
+        <v>251227</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D21" t="n">
-        <v>422.5211267605634</v>
+        <v>0</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-08 12:37:35</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-08 12:17:00</t>
+          <t>2025-05-08 12:52:35</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-08 12:17:00</t>
+          <t>2025-05-08 12:52:35</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-09 11:19:31</t>
+          <t>2025-05-08 12:52:35</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>29999</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2027,17 +2027,17 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M21" t="n">
         <v>76</v>
       </c>
       <c r="N21" t="n">
-        <v>39760</v>
+        <v>39746</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2045,57 +2045,57 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>39760</v>
+        <v>39746</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R21" s="1" t="n">
-        <v>-2.471889671365741</v>
+        <v>-2.5365234375</v>
       </c>
       <c r="S21" s="1" t="n">
-        <v>-2.471889671365741</v>
+        <v>-2.5365234375</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>251050</v>
+        <v>251421</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>217</v>
+        <v>17</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>81.9375</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 12:52:35</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 13:09:35</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 13:09:35</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 14:31:31</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>5244</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2104,17 +2104,19 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="M22" t="n">
-        <v>70</v>
-      </c>
-      <c r="N22" t="n">
-        <v>39747</v>
+        <v>76</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>39762 (non in estrazione)</t>
+        </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2122,57 +2124,57 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>39747</v>
+        <v>39762</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-08 00:00:00</t>
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>-0.6052300347222223</v>
       </c>
       <c r="S22" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>-0.6052300347222223</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251054</v>
+        <v>251782</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>188.640625</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 14:31:31</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-08 14:46:31</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-08 14:46:31</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-09 09:55:10</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>12073</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2181,17 +2183,17 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="M23" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N23" t="n">
-        <v>39747</v>
+        <v>39754</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2199,57 +2201,57 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>39747</v>
+        <v>39754</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>-0.4133138020833333</v>
       </c>
       <c r="S23" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>-0.4133138020833333</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>251081</v>
+        <v>250894</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>125</v>
+        <v>19</v>
       </c>
       <c r="D24" t="n">
-        <v>42.42253521126761</v>
+        <v>691.59375</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-09 09:55:10</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-09 10:14:10</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-09 10:14:10</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-05-09 13:59:25</t>
+          <t>2025-05-12 13:45:45</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>3012</v>
+        <v>44262</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2258,106 +2260,106 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="M24" t="n">
-        <v>70</v>
-      </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>39750 (esterno)</t>
-        </is>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N24" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
       </c>
       <c r="P24" t="n">
-        <v>39750</v>
+        <v>0</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R24" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>0</v>
       </c>
       <c r="S24" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>251651</v>
+        <v>251706</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>767.7049180327868</v>
+        <v>50.79365079365079</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-12 12:16:42</t>
+          <t>2025-05-12 07:50:47</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>46830</v>
+        <v>3200</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>bobina</t>
+          <t>foglio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
-        <v>76</v>
-      </c>
-      <c r="N25" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O25" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>39764 (esterno)</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P25" t="n">
-        <v>0</v>
+        <v>39764</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-05-14 00:00:00</t>
         </is>
       </c>
       <c r="R25" s="1" t="n">
@@ -2369,41 +2371,41 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251742</v>
+        <v>251050</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>30</v>
+        <v>217</v>
       </c>
       <c r="D26" t="n">
-        <v>134.8524590163935</v>
+        <v>0</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>8226</v>
+        <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2412,17 +2414,17 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="M26" t="n">
         <v>70</v>
       </c>
       <c r="N26" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2430,57 +2432,57 @@
         </is>
       </c>
       <c r="P26" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R26" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-1.442361111111111</v>
       </c>
       <c r="S26" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-1.442361111111111</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251840</v>
+        <v>251054</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D27" t="n">
-        <v>93.67213114754098</v>
+        <v>0</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>5714</v>
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2489,17 +2491,17 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="M27" t="n">
         <v>70</v>
       </c>
       <c r="N27" t="n">
-        <v>39758</v>
+        <v>39747</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2507,57 +2509,57 @@
         </is>
       </c>
       <c r="P27" t="n">
-        <v>39758</v>
+        <v>39747</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R27" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>-1.466666666666667</v>
       </c>
       <c r="S27" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>-1.466666666666667</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>251456</v>
+        <v>251081</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="D28" t="n">
-        <v>147.5245901639344</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-05-08 12:13:31</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-05-08 12:13:31</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-05-08 14:41:02</t>
+          <t>2025-05-09 13:59:25</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>8999</v>
+        <v>3012</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2566,17 +2568,19 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L28" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="M28" t="n">
         <v>70</v>
       </c>
-      <c r="N28" t="n">
-        <v>39746</v>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>39750 (esterno)</t>
+        </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2584,57 +2588,57 @@
         </is>
       </c>
       <c r="P28" t="n">
-        <v>39746</v>
+        <v>39750</v>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R28" s="1" t="n">
-        <v>-2.611839708564815</v>
+        <v>-16.58293231612268</v>
       </c>
       <c r="S28" s="1" t="n">
-        <v>-2.611839708564815</v>
+        <v>-16.58293231612268</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>251268</v>
+        <v>251284</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>47</v>
+        <v>40.5</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>16340</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2643,19 +2647,17 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L29" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M29" t="n">
-        <v>76</v>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>39666 (non in estrazione)</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="N29" t="n">
+        <v>39747</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2663,57 +2665,57 @@
         </is>
       </c>
       <c r="P29" t="n">
-        <v>39666</v>
+        <v>39747</v>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>2025-04-14 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R29" s="1" t="n">
-        <v>-24.32430555555555</v>
+        <v>-1.526104797974537</v>
       </c>
       <c r="S29" s="1" t="n">
-        <v>-24.32430555555555</v>
+        <v>-1.526104797974537</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>251164</v>
+        <v>251651</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D30" t="n">
-        <v>204.0816326530612</v>
+        <v>767.7049180327868</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-05-08 08:34:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-05-08 08:34:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-05-08 11:58:04</t>
+          <t>2025-05-12 12:16:42</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>10000</v>
+        <v>46830</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2722,36 +2724,34 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M30" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N30" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
       </c>
       <c r="P30" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R30" s="1" t="n">
-        <v>-1.498667800451389</v>
+        <v>0</v>
       </c>
       <c r="S30" s="1" t="n">
-        <v>-1.498667800451389</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">

</xml_diff>

<commit_message>
Rimesso check a inizio_lavorazione anziché fine_lavorazione sulla release date per le ricerche locali
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_post.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_post.xlsx
@@ -1287,41 +1287,41 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251455</v>
+        <v>251651</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D12" t="n">
-        <v>82.765625</v>
+        <v>767.7049180327868</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-07 07:00:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-07 08:41:45</t>
+          <t>2025-05-12 12:16:42</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>5297</v>
+        <v>46830</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1330,41 +1330,39 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M12" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N12" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-04-15 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>-0.3623372395833334</v>
+        <v>0</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>-0.3623372395833334</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251391</v>
+        <v>251455</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1372,33 +1370,33 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D13" t="n">
-        <v>91.640625</v>
+        <v>82.765625</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
+          <t>2025-05-07 07:00:00</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-05-07 07:19:00</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2025-05-07 07:19:00</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
           <t>2025-05-07 08:41:45</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>2025-05-07 08:58:45</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>2025-05-07 08:58:45</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>2025-05-07 10:30:24</t>
-        </is>
-      </c>
       <c r="I13" t="n">
-        <v>5865</v>
+        <v>5297</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1411,7 +1409,7 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M13" t="n">
         <v>70</v>
@@ -1429,19 +1427,19 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-15 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-0.4377821180555556</v>
+        <v>-0.3623372395833334</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>-0.4377821180555556</v>
+        <v>-0.3623372395833334</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>251395</v>
+        <v>251391</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1452,30 +1450,30 @@
         <v>17</v>
       </c>
       <c r="D14" t="n">
-        <v>35.34375</v>
+        <v>91.640625</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
+          <t>2025-05-07 08:41:45</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-05-07 08:58:45</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2025-05-07 08:58:45</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
           <t>2025-05-07 10:30:24</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2025-05-07 10:47:24</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>2025-05-07 10:47:24</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>2025-05-07 11:22:45</t>
-        </is>
-      </c>
       <c r="I14" t="n">
-        <v>2262</v>
+        <v>5865</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1488,7 +1486,7 @@
         </is>
       </c>
       <c r="L14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M14" t="n">
         <v>70</v>
@@ -1510,15 +1508,15 @@
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-0.4741319444444445</v>
+        <v>-0.4377821180555556</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>-0.4741319444444445</v>
+        <v>-0.4377821180555556</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>251371</v>
+        <v>251395</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1526,33 +1524,33 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>35.34375</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
+          <t>2025-05-07 10:30:24</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-05-07 10:47:24</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2025-05-07 10:47:24</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
           <t>2025-05-07 11:22:45</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2025-05-07 11:41:45</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2025-05-07 11:41:45</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>2025-05-07 11:41:45</t>
-        </is>
-      </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>2262</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1565,15 +1563,13 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M15" t="n">
         <v>70</v>
       </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>39666 (esterno)</t>
-        </is>
+      <c r="N15" t="n">
+        <v>39749</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1581,23 +1577,23 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>39666</v>
+        <v>39749</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-04-24 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-13.48732638888889</v>
+        <v>-0.4741319444444445</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>-13.48732638888889</v>
+        <v>-0.4741319444444445</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251453</v>
+        <v>251371</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1605,33 +1601,33 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D16" t="n">
-        <v>78.125</v>
+        <v>0</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
+          <t>2025-05-07 11:22:45</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
           <t>2025-05-07 11:41:45</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2025-05-07 11:58:45</t>
-        </is>
-      </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-07 11:58:45</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-07 13:16:52</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1644,14 +1640,14 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M16" t="n">
         <v>70</v>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>39742 (non in estrazione)</t>
+          <t>39666 (esterno)</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -1660,23 +1656,23 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>39742</v>
+        <v>39666</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-04-24 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-9.553385416666666</v>
+        <v>-13.48732638888889</v>
       </c>
       <c r="S16" s="1" t="n">
-        <v>-9.553385416666666</v>
+        <v>-13.48732638888889</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251396</v>
+        <v>251453</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1684,33 +1680,33 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D17" t="n">
-        <v>35.34375</v>
+        <v>78.125</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
+          <t>2025-05-07 11:41:45</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-05-07 11:58:45</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2025-05-07 11:58:45</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
           <t>2025-05-07 13:16:52</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2025-05-07 13:37:52</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>2025-05-07 13:37:52</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>2025-05-07 14:13:13</t>
-        </is>
-      </c>
       <c r="I17" t="n">
-        <v>2262</v>
+        <v>5000</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1723,13 +1719,15 @@
         </is>
       </c>
       <c r="L17" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M17" t="n">
         <v>70</v>
       </c>
-      <c r="N17" t="n">
-        <v>39749</v>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>39742 (non in estrazione)</t>
+        </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1737,23 +1735,23 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>39749</v>
+        <v>39742</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>-0.5925130208333333</v>
+        <v>-9.553385416666666</v>
       </c>
       <c r="S17" s="1" t="n">
-        <v>-0.5925130208333333</v>
+        <v>-9.553385416666666</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251548</v>
+        <v>251396</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1761,33 +1759,33 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D18" t="n">
-        <v>206.90625</v>
+        <v>35.34375</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
+          <t>2025-05-07 13:16:52</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-05-07 13:37:52</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2025-05-07 13:37:52</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
           <t>2025-05-07 14:13:13</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2025-05-07 14:32:13</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>2025-05-07 14:32:13</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>2025-05-08 09:59:07</t>
-        </is>
-      </c>
       <c r="I18" t="n">
-        <v>13242</v>
+        <v>2262</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1800,7 +1798,7 @@
         </is>
       </c>
       <c r="L18" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M18" t="n">
         <v>70</v>
@@ -1818,19 +1816,19 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-05-02 00:00:00</t>
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>-1.416059027777778</v>
+        <v>-0.5925130208333333</v>
       </c>
       <c r="S18" s="1" t="n">
-        <v>-1.416059027777778</v>
+        <v>-0.5925130208333333</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>250923</v>
+        <v>251548</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1838,33 +1836,33 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D19" t="n">
-        <v>109.46875</v>
+        <v>206.90625</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
+          <t>2025-05-07 14:13:13</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-05-07 14:32:13</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2025-05-07 14:32:13</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
           <t>2025-05-08 09:59:07</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2025-05-08 10:31:07</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>2025-05-08 10:31:07</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>2025-05-08 12:20:35</t>
-        </is>
-      </c>
       <c r="I19" t="n">
-        <v>7006</v>
+        <v>13242</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1873,14 +1871,14 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M19" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N19" t="n">
         <v>39749</v>
@@ -1895,19 +1893,19 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R19" s="1" t="n">
-        <v>-1.514301215277778</v>
+        <v>-1.416059027777778</v>
       </c>
       <c r="S19" s="1" t="n">
-        <v>-1.514301215277778</v>
+        <v>-1.416059027777778</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251225</v>
+        <v>250923</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1915,33 +1913,33 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>109.46875</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
+          <t>2025-05-08 09:59:07</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-05-08 10:31:07</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2025-05-08 10:31:07</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
           <t>2025-05-08 12:20:35</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>2025-05-08 12:37:35</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>2025-05-08 12:37:35</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>2025-05-08 12:37:35</t>
-        </is>
-      </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>7006</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1954,13 +1952,13 @@
         </is>
       </c>
       <c r="L20" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M20" t="n">
         <v>76</v>
       </c>
       <c r="N20" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1968,23 +1966,23 @@
         </is>
       </c>
       <c r="P20" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-04-07 00:00:00</t>
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>-0.5261067708333333</v>
+        <v>-1.514301215277778</v>
       </c>
       <c r="S20" s="1" t="n">
-        <v>-0.5261067708333333</v>
+        <v>-1.514301215277778</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251227</v>
+        <v>251225</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1992,29 +1990,29 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
+          <t>2025-05-08 12:20:35</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
           <t>2025-05-08 12:37:35</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2025-05-08 12:52:35</t>
-        </is>
-      </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-08 12:37:35</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-08 12:37:35</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2037,7 +2035,7 @@
         <v>76</v>
       </c>
       <c r="N21" t="n">
-        <v>39746</v>
+        <v>39747</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2045,23 +2043,23 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>39746</v>
+        <v>39747</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R21" s="1" t="n">
-        <v>-2.5365234375</v>
+        <v>-0.5261067708333333</v>
       </c>
       <c r="S21" s="1" t="n">
-        <v>-2.5365234375</v>
+        <v>-0.5261067708333333</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>251421</v>
+        <v>251227</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2069,33 +2067,33 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D22" t="n">
-        <v>81.9375</v>
+        <v>0</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
+          <t>2025-05-08 12:37:35</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
           <t>2025-05-08 12:52:35</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>2025-05-08 13:09:35</t>
-        </is>
-      </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-08 13:09:35</t>
+          <t>2025-05-08 12:52:35</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-08 14:31:31</t>
+          <t>2025-05-08 12:52:35</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>5244</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2104,19 +2102,17 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M22" t="n">
         <v>76</v>
       </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>39762 (non in estrazione)</t>
-        </is>
+      <c r="N22" t="n">
+        <v>39746</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2124,23 +2120,23 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>39762</v>
+        <v>39746</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2025-05-08 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>-0.6052300347222223</v>
+        <v>-2.5365234375</v>
       </c>
       <c r="S22" s="1" t="n">
-        <v>-0.6052300347222223</v>
+        <v>-2.5365234375</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251782</v>
+        <v>251421</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2148,33 +2144,33 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D23" t="n">
-        <v>188.640625</v>
+        <v>81.9375</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
+          <t>2025-05-08 12:52:35</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-05-08 13:09:35</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2025-05-08 13:09:35</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
           <t>2025-05-08 14:31:31</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>2025-05-08 14:46:31</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>2025-05-08 14:46:31</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>2025-05-09 09:55:10</t>
-        </is>
-      </c>
       <c r="I23" t="n">
-        <v>12073</v>
+        <v>5244</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2192,8 +2188,10 @@
       <c r="M23" t="n">
         <v>76</v>
       </c>
-      <c r="N23" t="n">
-        <v>39754</v>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>39762 (non in estrazione)</t>
+        </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2201,23 +2199,23 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>39754</v>
+        <v>39762</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-05-08 00:00:00</t>
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>-0.4133138020833333</v>
+        <v>-0.6052300347222223</v>
       </c>
       <c r="S23" s="1" t="n">
-        <v>-0.4133138020833333</v>
+        <v>-0.6052300347222223</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>250894</v>
+        <v>251782</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2225,33 +2223,33 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D24" t="n">
-        <v>691.59375</v>
+        <v>188.640625</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
+          <t>2025-05-08 14:31:31</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-05-08 14:46:31</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2025-05-08 14:46:31</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
           <t>2025-05-09 09:55:10</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>2025-05-09 10:14:10</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>2025-05-09 10:14:10</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>2025-05-12 13:45:45</t>
-        </is>
-      </c>
       <c r="I24" t="n">
-        <v>44262</v>
+        <v>12073</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2260,106 +2258,104 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M24" t="n">
         <v>76</v>
       </c>
       <c r="N24" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O24" t="n">
-        <v>0</v>
+        <v>39754</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P24" t="n">
-        <v>0</v>
+        <v>39754</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R24" s="1" t="n">
-        <v>0</v>
+        <v>-0.4133138020833333</v>
       </c>
       <c r="S24" s="1" t="n">
-        <v>0</v>
+        <v>-0.4133138020833333</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>251706</v>
+        <v>250894</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D25" t="n">
-        <v>50.79365079365079</v>
+        <v>691.59375</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-09 09:55:10</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-09 10:14:10</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-09 10:14:10</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-12 07:50:47</t>
+          <t>2025-05-12 13:45:45</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>3200</v>
+        <v>44262</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>foglio</t>
+          <t>bobina</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M25" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>39764 (esterno)</t>
-        </is>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N25" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
       </c>
       <c r="P25" t="n">
-        <v>39764</v>
+        <v>0</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2025-05-14 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R25" s="1" t="n">
@@ -2371,60 +2367,62 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251050</v>
+        <v>251706</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>217</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>50.79365079365079</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-12 07:50:47</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>3200</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>bobina</t>
+          <t>foglio</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="M26" t="n">
-        <v>70</v>
-      </c>
-      <c r="N26" t="n">
-        <v>39747</v>
+        <v>0</v>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>39764 (esterno)</t>
+        </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2432,23 +2430,23 @@
         </is>
       </c>
       <c r="P26" t="n">
-        <v>39747</v>
+        <v>39764</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-14 00:00:00</t>
         </is>
       </c>
       <c r="R26" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>0</v>
       </c>
       <c r="S26" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251054</v>
+        <v>251050</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -2456,29 +2454,29 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>35</v>
+        <v>217</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
+          <t>2025-05-09 07:00:00</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
           <t>2025-05-09 10:37:00</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>2025-05-09 11:12:00</t>
-        </is>
-      </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2517,15 +2515,15 @@
         </is>
       </c>
       <c r="R27" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>-1.442361111111111</v>
       </c>
       <c r="S27" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>-1.442361111111111</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>251081</v>
+        <v>251054</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2533,33 +2531,33 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>125</v>
+        <v>35</v>
       </c>
       <c r="D28" t="n">
-        <v>42.42253521126761</v>
+        <v>0</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
+          <t>2025-05-09 10:37:00</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
           <t>2025-05-09 11:12:00</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>2025-05-09 13:17:00</t>
-        </is>
-      </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-05-09 13:59:25</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>3012</v>
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2572,15 +2570,13 @@
         </is>
       </c>
       <c r="L28" t="n">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="M28" t="n">
         <v>70</v>
       </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>39750 (esterno)</t>
-        </is>
+      <c r="N28" t="n">
+        <v>39747</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2588,57 +2584,57 @@
         </is>
       </c>
       <c r="P28" t="n">
-        <v>39750</v>
+        <v>39747</v>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R28" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>-1.466666666666667</v>
       </c>
       <c r="S28" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>-1.466666666666667</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>251284</v>
+        <v>251081</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>40.5</v>
+        <v>125</v>
       </c>
       <c r="D29" t="n">
-        <v>297.0909090909091</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-09 13:59:25</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>16340</v>
+        <v>3012</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2647,17 +2643,19 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L29" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="M29" t="n">
         <v>70</v>
       </c>
-      <c r="N29" t="n">
-        <v>39747</v>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>39750 (esterno)</t>
+        </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2665,34 +2663,34 @@
         </is>
       </c>
       <c r="P29" t="n">
-        <v>39747</v>
+        <v>39750</v>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R29" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>-16.58293231612268</v>
       </c>
       <c r="S29" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>-16.58293231612268</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>251651</v>
+        <v>251284</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>29</v>
+        <v>40.5</v>
       </c>
       <c r="D30" t="n">
-        <v>767.7049180327868</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -2701,21 +2699,21 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-05-12 12:16:42</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>46830</v>
+        <v>16340</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2724,23 +2722,25 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L30" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M30" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N30" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O30" t="n">
-        <v>0</v>
+        <v>39747</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P30" t="n">
-        <v>0</v>
+        <v>39747</v>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
@@ -2748,10 +2748,10 @@
         </is>
       </c>
       <c r="R30" s="1" t="n">
-        <v>0</v>
+        <v>-1.526104797974537</v>
       </c>
       <c r="S30" s="1" t="n">
-        <v>0</v>
+        <v>-1.526104797974537</v>
       </c>
     </row>
     <row r="31">

</xml_diff>

<commit_message>
Cambio destianzione output / archiviazione output inutili
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_post.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_post.xlsx
@@ -515,60 +515,62 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251547</v>
+        <v>251706</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>184.9154929577465</v>
+        <v>50.79365079365079</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-12 07:50:47</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>13129</v>
+        <v>3200</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>bobina</t>
+          <t>foglio</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>70</v>
-      </c>
-      <c r="N2" t="n">
-        <v>39749</v>
+        <v>0</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>39764 (esterno)</t>
+        </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -576,57 +578,57 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>39749</v>
+        <v>39764</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-05-14 00:00:00</t>
         </is>
       </c>
       <c r="R2" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>0</v>
       </c>
       <c r="S2" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>250759</v>
+        <v>251455</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D3" t="n">
-        <v>118.2816901408451</v>
+        <v>82.765625</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-07 07:00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-07 08:41:45</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>8398</v>
+        <v>5297</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -635,17 +637,17 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L3" t="n">
         <v>4</v>
       </c>
       <c r="M3" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N3" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -653,57 +655,57 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
+          <t>2025-04-15 00:00:00</t>
         </is>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-0.3623372395833334</v>
       </c>
       <c r="S3" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-0.3623372395833334</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251229</v>
+        <v>251391</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D4" t="n">
-        <v>263.9295774647887</v>
+        <v>91.640625</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-07 08:41:45</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-08 13:41:11</t>
+          <t>2025-05-07 08:58:45</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-08 13:41:11</t>
+          <t>2025-05-07 08:58:45</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-09 10:05:07</t>
+          <t>2025-05-07 10:30:24</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>18739</v>
+        <v>5865</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -712,19 +714,17 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M4" t="n">
         <v>70</v>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>39723 (esterno)</t>
-        </is>
+      <c r="N4" t="n">
+        <v>39749</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -732,57 +732,57 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>39723</v>
+        <v>39749</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R4" s="1" t="n">
-        <v>0</v>
+        <v>-0.4377821180555556</v>
       </c>
       <c r="S4" s="1" t="n">
-        <v>0</v>
+        <v>-0.4377821180555556</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251416</v>
+        <v>251395</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D5" t="n">
-        <v>158.056338028169</v>
+        <v>35.34375</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-09 10:05:07</t>
+          <t>2025-05-07 10:30:24</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-09 10:28:07</t>
+          <t>2025-05-07 10:47:24</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-09 10:28:07</t>
+          <t>2025-05-07 10:47:24</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-09 13:06:10</t>
+          <t>2025-05-07 11:22:45</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>11222</v>
+        <v>2262</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -795,19 +795,21 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M5" t="n">
         <v>70</v>
       </c>
       <c r="N5" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
+        <v>39749</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>39749</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
@@ -815,49 +817,49 @@
         </is>
       </c>
       <c r="R5" s="1" t="n">
-        <v>0</v>
+        <v>-0.4741319444444445</v>
       </c>
       <c r="S5" s="1" t="n">
-        <v>0</v>
+        <v>-0.4741319444444445</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251742</v>
+        <v>251371</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D6" t="n">
-        <v>134.8524590163935</v>
+        <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-07 11:22:45</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>8226</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -875,8 +877,10 @@
       <c r="M6" t="n">
         <v>70</v>
       </c>
-      <c r="N6" t="n">
-        <v>39749</v>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>39666 (esterno)</t>
+        </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -884,57 +888,57 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>39749</v>
+        <v>39666</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-24 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-13.48732638888889</v>
       </c>
       <c r="S6" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-13.48732638888889</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251840</v>
+        <v>251453</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D7" t="n">
-        <v>93.67213114754098</v>
+        <v>78.125</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-07 11:58:45</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-07 11:58:45</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-07 13:16:52</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>5714</v>
+        <v>5000</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -947,13 +951,15 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M7" t="n">
         <v>70</v>
       </c>
-      <c r="N7" t="n">
-        <v>39758</v>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>39742 (non in estrazione)</t>
+        </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -961,57 +967,57 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>39758</v>
+        <v>39742</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>-9.553385416666666</v>
       </c>
       <c r="S7" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>-9.553385416666666</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251456</v>
+        <v>251396</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D8" t="n">
-        <v>147.5245901639344</v>
+        <v>35.34375</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-07 13:16:52</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-08 12:13:31</t>
+          <t>2025-05-07 13:37:52</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-08 12:13:31</t>
+          <t>2025-05-07 13:37:52</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-08 14:41:02</t>
+          <t>2025-05-07 14:13:13</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>8999</v>
+        <v>2262</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1024,13 +1030,13 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M8" t="n">
         <v>70</v>
       </c>
       <c r="N8" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1038,57 +1044,57 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-02 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>-2.611839708564815</v>
+        <v>-0.5925130208333333</v>
       </c>
       <c r="S8" s="1" t="n">
-        <v>-2.611839708564815</v>
+        <v>-0.5925130208333333</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251477</v>
+        <v>251548</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D9" t="n">
-        <v>422.5211267605634</v>
+        <v>206.90625</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-07 14:13:13</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-08 12:17:00</t>
+          <t>2025-05-07 14:32:13</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-08 12:17:00</t>
+          <t>2025-05-07 14:32:13</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-09 11:19:31</t>
+          <t>2025-05-08 09:59:07</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>29999</v>
+        <v>13242</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1097,17 +1103,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M9" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N9" t="n">
-        <v>39760</v>
+        <v>39749</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1115,57 +1121,57 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>39760</v>
+        <v>39749</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-2.471889671365741</v>
+        <v>-1.416059027777778</v>
       </c>
       <c r="S9" s="1" t="n">
-        <v>-2.471889671365741</v>
+        <v>-1.416059027777778</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251268</v>
+        <v>250923</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>109.46875</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-08 09:59:07</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-08 10:31:07</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-08 10:31:07</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-08 12:20:35</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>7006</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1174,19 +1180,17 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M10" t="n">
         <v>76</v>
       </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>39666 (non in estrazione)</t>
-        </is>
+      <c r="N10" t="n">
+        <v>39749</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1194,57 +1198,57 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>39666</v>
+        <v>39749</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-04-14 00:00:00</t>
+          <t>2025-04-07 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-24.32430555555555</v>
+        <v>-1.514301215277778</v>
       </c>
       <c r="S10" s="1" t="n">
-        <v>-24.32430555555555</v>
+        <v>-1.514301215277778</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251164</v>
+        <v>251225</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="D11" t="n">
-        <v>204.0816326530612</v>
+        <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-08 12:20:35</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-08 08:34:00</t>
+          <t>2025-05-08 12:37:35</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-08 08:34:00</t>
+          <t>2025-05-08 12:37:35</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-08 11:58:04</t>
+          <t>2025-05-08 12:37:35</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1253,17 +1257,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M11" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N11" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1271,57 +1275,57 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-1.498667800451389</v>
+        <v>-0.5261067708333333</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>-1.498667800451389</v>
+        <v>-0.5261067708333333</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251651</v>
+        <v>251227</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D12" t="n">
-        <v>767.7049180327868</v>
+        <v>0</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 12:37:35</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-08 12:52:35</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-08 12:52:35</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-12 12:16:42</t>
+          <t>2025-05-08 12:52:35</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>46830</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1330,39 +1334,41 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M12" t="n">
         <v>76</v>
       </c>
       <c r="N12" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0</v>
+        <v>39746</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>39746</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>0</v>
+        <v>-2.5365234375</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>0</v>
+        <v>-2.5365234375</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251455</v>
+        <v>251421</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1370,33 +1376,33 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" t="n">
-        <v>82.765625</v>
+        <v>81.9375</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-07 07:00:00</t>
+          <t>2025-05-08 12:52:35</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-08 13:09:35</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-08 13:09:35</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-07 08:41:45</t>
+          <t>2025-05-08 14:31:31</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>5297</v>
+        <v>5244</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1405,17 +1411,19 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M13" t="n">
-        <v>70</v>
-      </c>
-      <c r="N13" t="n">
-        <v>39749</v>
+        <v>76</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>39762 (non in estrazione)</t>
+        </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1423,23 +1431,23 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39749</v>
+        <v>39762</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-04-15 00:00:00</t>
+          <t>2025-05-08 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-0.3623372395833334</v>
+        <v>-0.6052300347222223</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>-0.3623372395833334</v>
+        <v>-0.6052300347222223</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>251391</v>
+        <v>251782</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1447,33 +1455,33 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D14" t="n">
-        <v>91.640625</v>
+        <v>188.640625</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-07 08:41:45</t>
+          <t>2025-05-08 14:31:31</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-07 08:58:45</t>
+          <t>2025-05-08 14:46:31</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-07 08:58:45</t>
+          <t>2025-05-08 14:46:31</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-07 10:30:24</t>
+          <t>2025-05-09 09:55:10</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>5865</v>
+        <v>12073</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1482,17 +1490,17 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M14" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N14" t="n">
-        <v>39749</v>
+        <v>39754</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1500,23 +1508,23 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>39749</v>
+        <v>39754</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-0.4377821180555556</v>
+        <v>-0.4133138020833333</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>-0.4377821180555556</v>
+        <v>-0.4133138020833333</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>251395</v>
+        <v>250894</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1524,33 +1532,33 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D15" t="n">
-        <v>35.34375</v>
+        <v>691.59375</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-07 10:30:24</t>
+          <t>2025-05-09 09:55:10</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-07 10:47:24</t>
+          <t>2025-05-09 10:14:10</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-07 10:47:24</t>
+          <t>2025-05-09 10:14:10</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:45</t>
+          <t>2025-05-12 13:45:45</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>2262</v>
+        <v>44262</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1559,71 +1567,69 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M15" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N15" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-0.4741319444444445</v>
+        <v>0</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>-0.4741319444444445</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251371</v>
+        <v>251050</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>19</v>
+        <v>217</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:45</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1636,19 +1642,17 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="M16" t="n">
         <v>70</v>
       </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>39666 (esterno)</t>
-        </is>
+      <c r="N16" t="n">
+        <v>39747</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1656,57 +1660,57 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>39666</v>
+        <v>39747</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-04-24 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-13.48732638888889</v>
+        <v>-1.442361111111111</v>
       </c>
       <c r="S16" s="1" t="n">
-        <v>-13.48732638888889</v>
+        <v>-1.442361111111111</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251453</v>
+        <v>251054</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D17" t="n">
-        <v>78.125</v>
+        <v>0</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-07 11:58:45</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-07 11:58:45</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-07 13:16:52</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1715,19 +1719,17 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="M17" t="n">
         <v>70</v>
       </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>39742 (non in estrazione)</t>
-        </is>
+      <c r="N17" t="n">
+        <v>39747</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1735,57 +1737,57 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>39742</v>
+        <v>39747</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>-9.553385416666666</v>
+        <v>-1.466666666666667</v>
       </c>
       <c r="S17" s="1" t="n">
-        <v>-9.553385416666666</v>
+        <v>-1.466666666666667</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251396</v>
+        <v>251081</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>21</v>
+        <v>125</v>
       </c>
       <c r="D18" t="n">
-        <v>35.34375</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-07 13:16:52</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-07 13:37:52</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-07 13:37:52</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-07 14:13:13</t>
+          <t>2025-05-09 13:59:25</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>2262</v>
+        <v>3012</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1794,17 +1796,19 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="M18" t="n">
         <v>70</v>
       </c>
-      <c r="N18" t="n">
-        <v>39749</v>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>39750 (esterno)</t>
+        </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1812,57 +1816,57 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>39749</v>
+        <v>39750</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>-0.5925130208333333</v>
+        <v>-16.58293231612268</v>
       </c>
       <c r="S18" s="1" t="n">
-        <v>-0.5925130208333333</v>
+        <v>-16.58293231612268</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251548</v>
+        <v>251284</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>19</v>
+        <v>40.5</v>
       </c>
       <c r="D19" t="n">
-        <v>206.90625</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-07 14:13:13</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-07 14:32:13</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-07 14:32:13</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-08 09:59:07</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>13242</v>
+        <v>16340</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1871,17 +1875,17 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M19" t="n">
         <v>70</v>
       </c>
       <c r="N19" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1889,57 +1893,57 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R19" s="1" t="n">
-        <v>-1.416059027777778</v>
+        <v>-1.526104797974537</v>
       </c>
       <c r="S19" s="1" t="n">
-        <v>-1.416059027777778</v>
+        <v>-1.526104797974537</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>250923</v>
+        <v>251742</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D20" t="n">
-        <v>109.46875</v>
+        <v>134.8524590163935</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-08 09:59:07</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-08 10:31:07</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-08 10:31:07</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-08 12:20:35</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>7006</v>
+        <v>8226</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1948,14 +1952,14 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M20" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N20" t="n">
         <v>39749</v>
@@ -1970,53 +1974,53 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>-1.514301215277778</v>
+        <v>-1.406147540983796</v>
       </c>
       <c r="S20" s="1" t="n">
-        <v>-1.514301215277778</v>
+        <v>-1.406147540983796</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251225</v>
+        <v>251840</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>93.67213114754098</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-08 12:20:35</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>5714</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2025,17 +2029,17 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M21" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N21" t="n">
-        <v>39747</v>
+        <v>39758</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2043,57 +2047,57 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>39747</v>
+        <v>39758</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R21" s="1" t="n">
-        <v>-0.5261067708333333</v>
+        <v>-0.4885587431712963</v>
       </c>
       <c r="S21" s="1" t="n">
-        <v>-0.5261067708333333</v>
+        <v>-0.4885587431712963</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>251227</v>
+        <v>251456</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>147.5245901639344</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-08 12:13:31</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-08 12:13:31</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-08 14:41:02</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>8999</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2102,14 +2106,14 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M22" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N22" t="n">
         <v>39746</v>
@@ -2124,53 +2128,53 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>-2.5365234375</v>
+        <v>-2.611839708564815</v>
       </c>
       <c r="S22" s="1" t="n">
-        <v>-2.5365234375</v>
+        <v>-2.611839708564815</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251421</v>
+        <v>251547</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D23" t="n">
-        <v>81.9375</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-08 13:09:35</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-08 13:09:35</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-08 14:31:31</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>5244</v>
+        <v>13129</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2179,19 +2183,17 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M23" t="n">
-        <v>76</v>
-      </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>39762 (non in estrazione)</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="N23" t="n">
+        <v>39749</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2199,57 +2201,57 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>39762</v>
+        <v>39749</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2025-05-08 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>-0.6052300347222223</v>
+        <v>-1.443691314548611</v>
       </c>
       <c r="S23" s="1" t="n">
-        <v>-0.6052300347222223</v>
+        <v>-1.443691314548611</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>251782</v>
+        <v>250759</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D24" t="n">
-        <v>188.640625</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-05-08 14:31:31</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-08 14:46:31</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-05-08 14:46:31</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-05-09 09:55:10</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>12073</v>
+        <v>8398</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2258,17 +2260,17 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M24" t="n">
         <v>76</v>
       </c>
       <c r="N24" t="n">
-        <v>39754</v>
+        <v>39747</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2276,57 +2278,57 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>39754</v>
+        <v>39747</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-03-13 00:00:00</t>
         </is>
       </c>
       <c r="R24" s="1" t="n">
-        <v>-0.4133138020833333</v>
+        <v>-0.5466647104861111</v>
       </c>
       <c r="S24" s="1" t="n">
-        <v>-0.4133138020833333</v>
+        <v>-0.5466647104861111</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>250894</v>
+        <v>251229</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D25" t="n">
-        <v>691.59375</v>
+        <v>263.9295774647887</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-05-09 09:55:10</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-09 10:14:10</t>
+          <t>2025-05-08 13:41:11</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-09 10:14:10</t>
+          <t>2025-05-08 13:41:11</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-12 13:45:45</t>
+          <t>2025-05-09 10:05:07</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>44262</v>
+        <v>18739</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2335,27 +2337,31 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M25" t="n">
-        <v>76</v>
-      </c>
-      <c r="N25" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O25" t="n">
-        <v>0</v>
+        <v>70</v>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P25" t="n">
-        <v>0</v>
+        <v>39723</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R25" s="1" t="n">
@@ -2367,74 +2373,70 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251706</v>
+        <v>251416</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D26" t="n">
-        <v>50.79365079365079</v>
+        <v>158.056338028169</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-09 10:05:07</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-09 10:28:07</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-09 10:28:07</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-12 07:50:47</t>
+          <t>2025-05-09 13:06:10</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>3200</v>
+        <v>11222</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>foglio</t>
+          <t>bobina</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M26" t="n">
-        <v>0</v>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>39764 (esterno)</t>
-        </is>
-      </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="N26" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
       </c>
       <c r="P26" t="n">
-        <v>39764</v>
+        <v>0</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2025-05-14 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R26" s="1" t="n">
@@ -2446,41 +2448,41 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251050</v>
+        <v>251477</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>217</v>
+        <v>17</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>422.5211267605634</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 12:17:00</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 12:17:00</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-09 11:19:31</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>29999</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2489,17 +2491,17 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="M27" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N27" t="n">
-        <v>39747</v>
+        <v>39760</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2507,57 +2509,57 @@
         </is>
       </c>
       <c r="P27" t="n">
-        <v>39747</v>
+        <v>39760</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R27" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>-2.471889671365741</v>
       </c>
       <c r="S27" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>-2.471889671365741</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>251054</v>
+        <v>251651</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>767.7049180327868</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-12 12:16:42</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>46830</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2566,75 +2568,73 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L28" t="n">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="M28" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N28" t="n">
-        <v>39747</v>
-      </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0</v>
       </c>
       <c r="P28" t="n">
-        <v>39747</v>
+        <v>0</v>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R28" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>0</v>
       </c>
       <c r="S28" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>251081</v>
+        <v>251268</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>125</v>
+        <v>47</v>
       </c>
       <c r="D29" t="n">
-        <v>42.42253521126761</v>
+        <v>0</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-08 07:47:00</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-08 07:47:00</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-05-09 13:59:25</t>
+          <t>2025-05-08 07:47:00</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>3012</v>
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2643,18 +2643,18 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L29" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="M29" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>39750 (esterno)</t>
+          <t>39666 (non in estrazione)</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
@@ -2663,57 +2663,57 @@
         </is>
       </c>
       <c r="P29" t="n">
-        <v>39750</v>
+        <v>39666</v>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-14 00:00:00</t>
         </is>
       </c>
       <c r="R29" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>-24.32430555555555</v>
       </c>
       <c r="S29" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>-24.32430555555555</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>251284</v>
+        <v>251164</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>40.5</v>
+        <v>47</v>
       </c>
       <c r="D30" t="n">
-        <v>297.0909090909091</v>
+        <v>204.0816326530612</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 07:47:00</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-08 08:34:00</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-08 08:34:00</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-08 11:58:04</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>16340</v>
+        <v>10000</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2722,17 +2722,17 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M30" t="n">
         <v>70</v>
       </c>
       <c r="N30" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2740,18 +2740,18 @@
         </is>
       </c>
       <c r="P30" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-04-22 00:00:00</t>
         </is>
       </c>
       <c r="R30" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>-1.498667800451389</v>
       </c>
       <c r="S30" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>-1.498667800451389</v>
       </c>
     </row>
     <row r="31">

</xml_diff>